<commit_message>
Assignments for the Coursera training
</commit_message>
<xml_diff>
--- a/NNML-Coursera-Training/TestsSheet.xlsx
+++ b/NNML-Coursera-Training/TestsSheet.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
     <sheet name="Tests" sheetId="3" r:id="rId2"/>
+    <sheet name="HotField" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
   <si>
     <t>SIGMOID</t>
   </si>
@@ -96,6 +97,18 @@
   </si>
   <si>
     <t>(w(xh)*x(t=2)) + (w(hh)*(h-2)) + b</t>
+  </si>
+  <si>
+    <t>b = 1</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>E = − Σ  si bi - Σ sisj wij</t>
   </si>
 </sst>
 </file>
@@ -136,7 +149,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,8 +186,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -430,15 +455,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -490,15 +551,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -524,23 +576,53 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -852,11 +934,11 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -919,7 +1001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
@@ -937,18 +1019,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="7">
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
         <f>1/(1+EXP(-M8))</f>
         <v>0.5</v>
       </c>
@@ -961,760 +1043,764 @@
     </row>
     <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19" t="s">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="K7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="14" t="s">
+      <c r="L7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="15" t="s">
+      <c r="M7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="23"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="12">
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="37"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="11">
         <f>1/(1+EXP(-M8))</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="25">
+      <c r="B9" s="28"/>
+      <c r="C9" s="21">
         <v>9</v>
       </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="27">
+      <c r="D9" s="33"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="23">
         <v>9</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="20">
         <v>9</v>
       </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="12">
+      <c r="J9" s="7"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="11">
         <f t="shared" ref="N9:N10" si="0">1/(1+EXP(-M9))</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="35">
-        <v>0.5</v>
-      </c>
-      <c r="E10" s="35"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="37"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="12">
+      <c r="B10" s="38"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="30"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="32"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="11">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="30" t="s">
+      <c r="B11" s="28"/>
+      <c r="C11" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="35"/>
-      <c r="E11" s="29">
+      <c r="D11" s="30"/>
+      <c r="E11" s="25">
         <v>-1</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="15">
         <f>N11</f>
         <v>0.97068776924864364</v>
       </c>
-      <c r="J11" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="K11" s="4">
+      <c r="J11" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="K11" s="3">
         <v>9</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="3">
         <v>-1</v>
       </c>
-      <c r="M11" s="11">
+      <c r="M11" s="10">
         <f t="shared" ref="M11" si="1">J11*K11+L11</f>
         <v>3.5</v>
       </c>
-      <c r="N11" s="12">
-        <f t="shared" ref="N11:N37" si="2">1/(1+EXP(-M11))</f>
+      <c r="N11" s="11">
+        <f t="shared" ref="N11:N36" si="2">1/(1+EXP(-M11))</f>
         <v>0.97068776924864364</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="35">
+      <c r="B12" s="38"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="30">
         <v>-1</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="16"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="11">
-        <f t="shared" ref="M12:M22" si="3">J12*K12+L12</f>
-        <v>0</v>
-      </c>
-      <c r="N12" s="12">
+      <c r="E12" s="25"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="15"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="10">
+        <f t="shared" ref="M12:M18" si="3">J12*K12+L12</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="11">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="23"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="11">
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="37"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N13" s="12">
+      <c r="N13" s="11">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="25">
+      <c r="B14" s="28"/>
+      <c r="C14" s="21">
         <v>4</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="27">
+      <c r="D14" s="33"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="23">
         <v>4</v>
       </c>
-      <c r="G14" s="24">
+      <c r="G14" s="20">
         <v>4</v>
       </c>
-      <c r="J14" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="K14" s="4">
+      <c r="J14" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="K14" s="3">
         <v>4</v>
       </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="11">
+      <c r="L14" s="3"/>
+      <c r="M14" s="10">
         <f>J14*K14</f>
         <v>2</v>
       </c>
-      <c r="N14" s="12"/>
+      <c r="N14" s="11"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="35">
-        <v>0.5</v>
-      </c>
-      <c r="E15" s="35"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="37"/>
-      <c r="J15" s="8">
+      <c r="B15" s="38"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="32"/>
+      <c r="J15" s="7">
         <v>-1</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="3">
         <f>G11</f>
         <v>0.97068776924864364</v>
       </c>
-      <c r="L15" s="4"/>
-      <c r="M15" s="11">
+      <c r="L15" s="3"/>
+      <c r="M15" s="10">
         <f>J15*K15</f>
         <v>-0.97068776924864364</v>
       </c>
-      <c r="N15" s="12"/>
+      <c r="N15" s="11"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="35">
+      <c r="B16" s="38"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="30">
         <v>-1</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="16"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="11">
+      <c r="E16" s="25"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="15"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N16" s="12">
+      <c r="N16" s="11">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="30" t="s">
+      <c r="B17" s="28"/>
+      <c r="C17" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="35"/>
-      <c r="E17" s="29">
+      <c r="D17" s="30"/>
+      <c r="E17" s="25">
         <v>-1</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17" s="15">
         <f>N17</f>
         <v>0.50732753303979039</v>
       </c>
-      <c r="J17" s="8"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4">
+      <c r="J17" s="7"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3">
         <v>-1</v>
       </c>
-      <c r="M17" s="11">
+      <c r="M17" s="10">
         <f>M14+M15+L17</f>
         <v>2.931223075135625E-2</v>
       </c>
-      <c r="N17" s="12">
+      <c r="N17" s="11">
         <f t="shared" si="2"/>
         <v>0.50732753303979039</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="23"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="11">
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="37"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N18" s="12">
+      <c r="N18" s="11">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="25">
+      <c r="B19" s="28"/>
+      <c r="C19" s="21">
         <v>-2</v>
       </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="25">
+      <c r="D19" s="33"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="21">
         <v>-2</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="21">
         <v>-2</v>
       </c>
-      <c r="J19" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="K19" s="4">
+      <c r="J19" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="K19" s="3">
         <v>-2</v>
       </c>
-      <c r="L19" s="4"/>
-      <c r="M19" s="11">
+      <c r="L19" s="3"/>
+      <c r="M19" s="10">
         <f>J19*K19</f>
         <v>-1</v>
       </c>
-      <c r="N19" s="12"/>
+      <c r="N19" s="11"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="35">
-        <v>0.5</v>
-      </c>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="37"/>
-      <c r="J20" s="8">
+      <c r="B20" s="38"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="30"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="32"/>
+      <c r="J20" s="7">
         <v>-1</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="3">
         <f>G17</f>
         <v>0.50732753303979039</v>
       </c>
-      <c r="L20" s="4"/>
-      <c r="M20" s="11">
+      <c r="L20" s="3"/>
+      <c r="M20" s="10">
         <f>J20*K20</f>
         <v>-0.50732753303979039</v>
       </c>
-      <c r="N20" s="12"/>
+      <c r="N20" s="11"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="35">
+      <c r="B21" s="38"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="30">
         <v>-1</v>
       </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="16"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="11">
+      <c r="E21" s="25"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="15"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="10">
         <f t="shared" ref="M21" si="4">J21*K21+L21</f>
         <v>0</v>
       </c>
-      <c r="N21" s="12">
+      <c r="N21" s="11">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="30" t="s">
+      <c r="B22" s="28"/>
+      <c r="C22" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="35"/>
-      <c r="E22" s="29">
+      <c r="D22" s="30"/>
+      <c r="E22" s="25">
         <v>-1</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F22" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="16">
+      <c r="G22" s="15">
         <f>N22</f>
         <v>7.5346086555395458E-2</v>
       </c>
-      <c r="J22" s="8"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4">
+      <c r="J22" s="7"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3">
         <v>-1</v>
       </c>
-      <c r="M22" s="11">
+      <c r="M22" s="10">
         <f>M19+M20+L22</f>
         <v>-2.5073275330397902</v>
       </c>
-      <c r="N22" s="12">
+      <c r="N22" s="11">
         <f>1/(1+EXP(-M22))</f>
         <v>7.5346086555395458E-2</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="35">
+      <c r="B23" s="38"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="30">
         <v>-0.7</v>
       </c>
-      <c r="E23" s="29"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="16"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="11">
+      <c r="E23" s="25"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="15"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="10">
         <f t="shared" ref="M23:M26" si="5">J23*K23+L23</f>
         <v>0</v>
       </c>
-      <c r="N23" s="12">
+      <c r="N23" s="11">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="32"/>
-      <c r="C24" s="30" t="s">
+      <c r="B24" s="28"/>
+      <c r="C24" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="35"/>
-      <c r="E24" s="29">
-        <v>0</v>
-      </c>
-      <c r="F24" s="17" t="s">
+      <c r="D24" s="30"/>
+      <c r="E24" s="25">
+        <v>0</v>
+      </c>
+      <c r="F24" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G24" s="16">
+      <c r="G24" s="15">
         <f>M24</f>
         <v>-5.2742260588776818E-2</v>
       </c>
-      <c r="J24" s="8">
+      <c r="J24" s="7">
         <v>-0.7</v>
       </c>
-      <c r="K24" s="4">
+      <c r="K24" s="3">
         <f>G22</f>
         <v>7.5346086555395458E-2</v>
       </c>
-      <c r="L24" s="4">
-        <v>0</v>
-      </c>
-      <c r="M24" s="11">
+      <c r="L24" s="3">
+        <v>0</v>
+      </c>
+      <c r="M24" s="10">
         <f t="shared" si="5"/>
         <v>-5.2742260588776818E-2</v>
       </c>
-      <c r="N24" s="12"/>
+      <c r="N24" s="11"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J25" s="8"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="11">
+      <c r="J25" s="7"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="10">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="N25" s="12">
+      <c r="N25" s="11">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J26" s="8"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="11">
+      <c r="J26" s="7"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="10">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="N26" s="12">
+      <c r="N26" s="11">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J27" s="8"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="11">
+      <c r="J27" s="7"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="10">
         <f t="shared" ref="M27:M37" si="6">J27*K27+L27</f>
         <v>0</v>
       </c>
-      <c r="N27" s="12">
+      <c r="N27" s="11">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J28" s="8"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="11">
+      <c r="J28" s="7"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N28" s="12">
+      <c r="N28" s="11">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J29" s="8"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="11">
+      <c r="J29" s="7"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N29" s="12">
+      <c r="N29" s="11">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J30" s="8"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="11">
+      <c r="J30" s="7"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N30" s="12">
+      <c r="N30" s="11">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="23"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="11">
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="37"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N31" s="12">
+      <c r="N31" s="11">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="32"/>
-      <c r="C32" s="25">
+      <c r="B32" s="28"/>
+      <c r="C32" s="21">
         <v>4</v>
       </c>
-      <c r="D32" s="38"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="27">
+      <c r="D32" s="33"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="23">
         <v>4</v>
       </c>
-      <c r="G32" s="24">
+      <c r="G32" s="20">
         <v>4</v>
       </c>
-      <c r="J32" s="8"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="11">
+      <c r="J32" s="7"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N32" s="12">
+      <c r="N32" s="11">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="33"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="35">
-        <v>0.5</v>
-      </c>
-      <c r="E33" s="35"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="37"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="11">
+      <c r="B33" s="38"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="E33" s="30"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="32"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N33" s="12">
+      <c r="N33" s="11">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
+      <c r="A34" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="33"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="35">
+      <c r="B34" s="38"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="30">
         <v>-1</v>
       </c>
-      <c r="E34" s="29"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="16"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="11">
+      <c r="E34" s="25"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="15"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N34" s="12">
+      <c r="N34" s="11">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="30" t="s">
+      <c r="B35" s="28"/>
+      <c r="C35" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="35"/>
-      <c r="E35" s="29">
+      <c r="D35" s="30"/>
+      <c r="E35" s="25">
         <v>-1</v>
       </c>
-      <c r="F35" s="17" t="s">
+      <c r="F35" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G35" s="16">
+      <c r="G35" s="15">
         <f>N17</f>
         <v>0.50732753303979039</v>
       </c>
-      <c r="J35" s="8"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="11">
+      <c r="J35" s="7"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N35" s="12">
+      <c r="N35" s="11">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="33" t="s">
+      <c r="A36" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="33"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="35">
+      <c r="B36" s="38"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="30">
         <v>-0.7</v>
       </c>
-      <c r="E36" s="29"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="16"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="11">
+      <c r="E36" s="25"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="15"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N36" s="12">
+      <c r="N36" s="11">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="32"/>
-      <c r="C37" s="30" t="s">
+      <c r="B37" s="28"/>
+      <c r="C37" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="35"/>
-      <c r="E37" s="29">
-        <v>0</v>
-      </c>
-      <c r="F37" s="17" t="s">
+      <c r="D37" s="30"/>
+      <c r="E37" s="25">
+        <v>0</v>
+      </c>
+      <c r="F37" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G37" s="16">
+      <c r="G37" s="15">
         <f>M37</f>
         <v>-0.35512927312785325</v>
       </c>
-      <c r="J37" s="8">
+      <c r="J37" s="7">
         <v>-0.7</v>
       </c>
-      <c r="K37" s="4">
+      <c r="K37" s="3">
         <f>G35</f>
         <v>0.50732753303979039</v>
       </c>
-      <c r="L37" s="4">
-        <v>0</v>
-      </c>
-      <c r="M37" s="11">
+      <c r="L37" s="3">
+        <v>0</v>
+      </c>
+      <c r="M37" s="10">
         <f t="shared" si="6"/>
         <v>-0.35512927312785325</v>
       </c>
-      <c r="N37" s="12"/>
+      <c r="N37" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:G13"/>
     <mergeCell ref="A31:G31"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
@@ -1725,11 +1811,95 @@
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D3:N23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="14" width="36.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="39"/>
+    </row>
+    <row r="5" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="F5" s="40"/>
+      <c r="L5" s="40"/>
+    </row>
+    <row r="6" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="F6" s="40"/>
+      <c r="L6" s="40"/>
+    </row>
+    <row r="7" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="40"/>
+      <c r="L7" s="40"/>
+    </row>
+    <row r="8" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="42">
+        <v>0</v>
+      </c>
+      <c r="I8" s="44">
+        <v>11</v>
+      </c>
+      <c r="L8" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="F9" s="40"/>
+      <c r="L9" s="40"/>
+    </row>
+    <row r="10" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="F10" s="40"/>
+      <c r="L10" s="40"/>
+    </row>
+    <row r="11" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="F11" s="40"/>
+      <c r="L11" s="40"/>
+    </row>
+    <row r="12" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="F12" s="40"/>
+      <c r="L12" s="40"/>
+    </row>
+    <row r="13" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" s="41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N23" s="46" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>